<commit_message>
aggiorna modifiche gestione titoli
</commit_message>
<xml_diff>
--- a/report/accounting/asset_management/schema titoli.xlsx
+++ b/report/accounting/asset_management/schema titoli.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaron.ploszaj\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\P\Universal Images\Universal\report\accounting\asset_management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D802BD7D-F516-49DB-B649-D19BF84C0055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E54ADD08-FE98-47E5-B5D2-F7B502EB3958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="3660" windowWidth="31140" windowHeight="14130" xr2:uid="{F3CD7890-2F1A-4DCC-A859-DA51742E909C}"/>
+    <workbookView xWindow="3690" yWindow="10970" windowWidth="28580" windowHeight="15640" xr2:uid="{F3CD7890-2F1A-4DCC-A859-DA51742E909C}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="15">
   <si>
     <t>spese</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>Account</t>
+  </si>
+  <si>
+    <t>prova dati 1</t>
+  </si>
+  <si>
+    <t>prova dati 2</t>
   </si>
 </sst>
 </file>
@@ -88,12 +94,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -108,8 +120,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -424,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F4E062F-3A88-4CED-BA9F-4C260A6C691F}">
-  <dimension ref="C5:I15"/>
+  <dimension ref="C4:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -439,8 +452,15 @@
     <col min="9" max="9" width="22.26953125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="4" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+    </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="E5" t="s">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G5" t="s">
@@ -448,13 +468,13 @@
       </c>
     </row>
     <row r="6" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>130000</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>1020</v>
       </c>
       <c r="G6" t="s">
@@ -464,17 +484,17 @@
         <v>9</v>
       </c>
       <c r="I6">
-        <v>130000</v>
+        <v>299000</v>
       </c>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>2000</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>6900</v>
       </c>
       <c r="G7" t="s">
@@ -485,13 +505,14 @@
       </c>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <f>D6+D7</f>
         <v>132000</v>
       </c>
+      <c r="E8" s="1"/>
       <c r="G8" t="s">
         <v>7</v>
       </c>
@@ -500,31 +521,33 @@
       </c>
       <c r="I8">
         <f>I6+I7</f>
-        <v>132000</v>
+        <v>301000</v>
       </c>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>10000</v>
       </c>
+      <c r="E9" s="1"/>
       <c r="G9" t="s">
         <v>1</v>
       </c>
       <c r="I9">
-        <v>10000</v>
+        <v>25000</v>
       </c>
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <f>D8/D9</f>
         <v>13.2</v>
       </c>
+      <c r="E10" s="1"/>
       <c r="G10" t="s">
         <v>2</v>
       </c>
@@ -533,16 +556,17 @@
       </c>
       <c r="I10">
         <f>I8/I9</f>
-        <v>13.2</v>
+        <v>12.04</v>
       </c>
     </row>
     <row r="11" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>13.8</v>
       </c>
+      <c r="E11" s="1"/>
       <c r="G11" t="s">
         <v>3</v>
       </c>
@@ -550,18 +574,23 @@
         <v>9</v>
       </c>
       <c r="I11">
-        <v>13.8</v>
-      </c>
+        <v>11.6</v>
+      </c>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <f>D11*D9</f>
         <v>138000</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="1">
         <v>1400</v>
       </c>
       <c r="G13" t="s">
@@ -572,18 +601,18 @@
       </c>
       <c r="I13">
         <f>I11*I9</f>
-        <v>138000</v>
+        <v>290000</v>
       </c>
     </row>
     <row r="14" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="1">
         <f>D8-D13</f>
         <v>-6000</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="1">
         <v>4200</v>
       </c>
       <c r="G14" t="s">
@@ -594,7 +623,7 @@
       </c>
       <c r="I14">
         <f>I8-I13</f>
-        <v>-6000</v>
+        <v>11000</v>
       </c>
     </row>
     <row r="15" spans="3:9" x14ac:dyDescent="0.35">
@@ -603,6 +632,107 @@
       </c>
       <c r="H15" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="1">
+        <v>510000</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1">
+        <v>4000</v>
+      </c>
+      <c r="E23" s="1">
+        <v>6900</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="1">
+        <f>D22+D23</f>
+        <v>514000</v>
+      </c>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1">
+        <v>40000</v>
+      </c>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C26" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="1">
+        <f>D24/D25</f>
+        <v>12.85</v>
+      </c>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="1">
+        <v>13.8</v>
+      </c>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C29" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="1">
+        <f>D27*D25</f>
+        <v>552000</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="1">
+        <f>D24-D29</f>
+        <v>-38000</v>
+      </c>
+      <c r="E30" s="1">
+        <v>4200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
aggiorna modifiche estensione titoli
</commit_message>
<xml_diff>
--- a/report/accounting/asset_management/schema titoli.xlsx
+++ b/report/accounting/asset_management/schema titoli.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\P\Universal Images\Universal\report\accounting\asset_management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E54ADD08-FE98-47E5-B5D2-F7B502EB3958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC7502D1-5FE4-4DD5-A4D2-7FDB7F09F640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3690" yWindow="10970" windowWidth="28580" windowHeight="15640" xr2:uid="{F3CD7890-2F1A-4DCC-A859-DA51742E909C}"/>
+    <workbookView xWindow="29650" yWindow="1420" windowWidth="33870" windowHeight="16640" xr2:uid="{F3CD7890-2F1A-4DCC-A859-DA51742E909C}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
+    <sheet name="esempi" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="52">
   <si>
     <t>spese</t>
   </si>
@@ -79,19 +80,154 @@
   </si>
   <si>
     <t>prova dati 2</t>
+  </si>
+  <si>
+    <t>Vend. 10000 azioni UBS</t>
+  </si>
+  <si>
+    <t>Vend. 10000 azioni UBS spese banca</t>
+  </si>
+  <si>
+    <t>Vend. 10000 azioni UBS perdita su vendita</t>
+  </si>
+  <si>
+    <t>Vend. azioni Unicredit</t>
+  </si>
+  <si>
+    <t>Vend. azioni Unicredit utile su vendita</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vend. azioni Unicredit spese banca </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EUR </t>
+  </si>
+  <si>
+    <t>Cambio utilizzato:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valore azioni al prezzo medio di acquisto </t>
+  </si>
+  <si>
+    <t xml:space="preserve">prezzo medio di acquisto </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cambio </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saldo del conto titoli </t>
+  </si>
+  <si>
+    <t xml:space="preserve">vendita al cambio contabile </t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">acquisto </t>
+  </si>
+  <si>
+    <t>qt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prezzo </t>
+  </si>
+  <si>
+    <t>moneta</t>
+  </si>
+  <si>
+    <t>totale</t>
+  </si>
+  <si>
+    <t>cambio</t>
+  </si>
+  <si>
+    <t>chf</t>
+  </si>
+  <si>
+    <t>unicredit</t>
+  </si>
+  <si>
+    <t>eur</t>
+  </si>
+  <si>
+    <t>utile vendita</t>
+  </si>
+  <si>
+    <t xml:space="preserve">costo medio </t>
+  </si>
+  <si>
+    <t>valore acquisto</t>
+  </si>
+  <si>
+    <t>utile/perdita di vendita</t>
+  </si>
+  <si>
+    <t>perdita vendita</t>
+  </si>
+  <si>
+    <t>utile vendita+utile cambio</t>
+  </si>
+  <si>
+    <t>valore contabile</t>
+  </si>
+  <si>
+    <t>cambio contabile</t>
+  </si>
+  <si>
+    <t>utile/perdita di cambio</t>
+  </si>
+  <si>
+    <t>perdita vendita+utile cambio</t>
+  </si>
+  <si>
+    <t>Altri esempi</t>
+  </si>
+  <si>
+    <t>Esempio base</t>
+  </si>
+  <si>
+    <t>utile vendita+perdita cambio</t>
+  </si>
+  <si>
+    <t>perdita vendita+perdita cambio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="172" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -120,9 +256,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" indent="12"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -437,27 +598,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F4E062F-3A88-4CED-BA9F-4C260A6C691F}">
-  <dimension ref="C4:I30"/>
+  <dimension ref="C3:L45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="22.6328125" customWidth="1"/>
+    <col min="3" max="3" width="35.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="14.6328125" customWidth="1"/>
-    <col min="7" max="7" width="38.1796875" customWidth="1"/>
-    <col min="8" max="8" width="22.90625" customWidth="1"/>
-    <col min="9" max="9" width="22.26953125" customWidth="1"/>
+    <col min="7" max="7" width="43.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.90625" customWidth="1"/>
+    <col min="9" max="10" width="22.26953125" customWidth="1"/>
+    <col min="11" max="11" width="19.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="7">
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
@@ -466,8 +636,17 @@
       <c r="G5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="I5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C6" s="1" t="s">
         <v>6</v>
       </c>
@@ -481,13 +660,16 @@
         <v>6</v>
       </c>
       <c r="H6" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="I6">
         <v>299000</v>
       </c>
-    </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="J6" s="7">
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C7" s="1" t="s">
         <v>0</v>
       </c>
@@ -500,11 +682,17 @@
       <c r="G7" t="s">
         <v>0</v>
       </c>
+      <c r="H7" t="s">
+        <v>9</v>
+      </c>
       <c r="I7">
         <v>2000</v>
       </c>
-    </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="J7" s="7">
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
@@ -523,8 +711,18 @@
         <f>I6+I7</f>
         <v>301000</v>
       </c>
-    </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.35">
+      <c r="J8" s="7">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="K8">
+        <f>I8*J8</f>
+        <v>346150</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C9" s="1" t="s">
         <v>1</v>
       </c>
@@ -539,7 +737,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C10" s="1" t="s">
         <v>2</v>
       </c>
@@ -559,7 +757,7 @@
         <v>12.04</v>
       </c>
     </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C11" s="1" t="s">
         <v>3</v>
       </c>
@@ -577,12 +775,12 @@
         <v>11.6</v>
       </c>
     </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C13" s="1" t="s">
         <v>5</v>
       </c>
@@ -604,7 +802,7 @@
         <v>290000</v>
       </c>
     </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C14" s="1" t="s">
         <v>4</v>
       </c>
@@ -625,117 +823,821 @@
         <f>I8-I13</f>
         <v>11000</v>
       </c>
-    </row>
-    <row r="15" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="G15" t="s">
+      <c r="J14">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="K14">
+        <f>J14*I14</f>
+        <v>12649.999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="G16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" t="s">
+        <v>9</v>
+      </c>
+      <c r="I16">
+        <v>580000</v>
+      </c>
+      <c r="J16" s="9">
+        <f>K16/I16</f>
+        <v>1.1086206896551725</v>
+      </c>
+      <c r="K16">
+        <v>643000</v>
+      </c>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="G17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H17" t="s">
+        <v>9</v>
+      </c>
+      <c r="I17">
+        <f>I8</f>
+        <v>301000</v>
+      </c>
+      <c r="J17" s="10">
+        <f>J16</f>
+        <v>1.1086206896551725</v>
+      </c>
+      <c r="K17" s="9">
+        <f>I17*J17</f>
+        <v>333694.8275862069</v>
+      </c>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="G18" t="s">
         <v>10</v>
       </c>
-      <c r="H15" t="s">
+      <c r="K18" s="9">
+        <f>K8-K17</f>
+        <v>12455.172413793101</v>
+      </c>
+      <c r="L18" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="1">
+        <v>5300</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="22" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1">
+        <v>200</v>
+      </c>
+      <c r="E22" s="1">
+        <v>6900</v>
+      </c>
+    </row>
+    <row r="23" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="1">
+        <f>D21+D22</f>
+        <v>5500</v>
+      </c>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1">
+        <v>500</v>
+      </c>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C25" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="1">
+        <f>D23/D24</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C22" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="1">
-        <v>510000</v>
-      </c>
-      <c r="E22" s="1">
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="1">
+        <v>10</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="G26" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H26" s="4">
+        <v>1024</v>
+      </c>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="3">
+        <v>299000</v>
+      </c>
+    </row>
+    <row r="27" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="G27" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H27" s="5"/>
+      <c r="I27" s="4">
+        <v>1402</v>
+      </c>
+      <c r="J27" s="4"/>
+      <c r="K27" s="3">
+        <v>289000</v>
+      </c>
+    </row>
+    <row r="28" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C28" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" s="1">
+        <f>D26*D24</f>
+        <v>5000</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1400</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H28" s="5"/>
+      <c r="I28" s="4">
+        <v>6900</v>
+      </c>
+      <c r="J28" s="4"/>
+      <c r="K28" s="3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="29" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="1">
+        <f>D23-D28</f>
+        <v>500</v>
+      </c>
+      <c r="E29" s="1">
+        <v>4200</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H29" s="5"/>
+      <c r="I29" s="4">
+        <v>3200</v>
+      </c>
+      <c r="J29" s="4"/>
+      <c r="K29" s="3">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="34" spans="7:11" x14ac:dyDescent="0.35">
+      <c r="G34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H34" s="4">
         <v>1020</v>
       </c>
-    </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C23" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D23" s="1">
-        <v>4000</v>
-      </c>
-      <c r="E23" s="1">
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="3">
+        <v>130000</v>
+      </c>
+    </row>
+    <row r="35" spans="7:11" x14ac:dyDescent="0.35">
+      <c r="G35" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H35" s="4">
         <v>6900</v>
       </c>
-    </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="1">
-        <f>D22+D23</f>
-        <v>514000</v>
-      </c>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C25" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D25" s="1">
-        <v>40000</v>
-      </c>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C26" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D26" s="1">
-        <f>D24/D25</f>
-        <v>12.85</v>
-      </c>
-      <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C27" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D27" s="1">
-        <v>13.8</v>
-      </c>
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C29" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" s="1">
-        <f>D27*D25</f>
-        <v>552000</v>
-      </c>
-      <c r="E29" s="1">
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="36" spans="7:11" x14ac:dyDescent="0.35">
+      <c r="G36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H36" s="4">
+        <v>4200</v>
+      </c>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="3">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="37" spans="7:11" x14ac:dyDescent="0.35">
+      <c r="G37" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H37" s="5"/>
+      <c r="I37" s="4">
         <v>1400</v>
       </c>
-    </row>
-    <row r="30" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C30" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" s="1">
-        <f>D24-D29</f>
-        <v>-38000</v>
-      </c>
-      <c r="E30" s="1">
-        <v>4200</v>
-      </c>
+      <c r="J37" s="4"/>
+      <c r="K37" s="3">
+        <v>138000</v>
+      </c>
+    </row>
+    <row r="38" spans="7:11" x14ac:dyDescent="0.35">
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6"/>
+    </row>
+    <row r="42" spans="7:11" x14ac:dyDescent="0.35">
+      <c r="G42" s="2"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="3"/>
+    </row>
+    <row r="43" spans="7:11" x14ac:dyDescent="0.35">
+      <c r="G43" s="2"/>
+      <c r="H43" s="4"/>
+      <c r="K43" s="3"/>
+    </row>
+    <row r="44" spans="7:11" x14ac:dyDescent="0.35">
+      <c r="G44" s="2"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="3"/>
+    </row>
+    <row r="45" spans="7:11" x14ac:dyDescent="0.35">
+      <c r="G45" s="2"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="4"/>
+      <c r="K45" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A615F4CA-572D-43F0-94F7-4A07CFE4C733}">
+  <dimension ref="B2:O19"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="27.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.36328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="C3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="O4" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5">
+        <v>100</v>
+      </c>
+      <c r="E5">
+        <v>100</v>
+      </c>
+      <c r="F5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5">
+        <f>E5*D5</f>
+        <v>10000</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <f>G5*H5</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>110</v>
+      </c>
+      <c r="F6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6">
+        <f>E6*D6</f>
+        <v>1100</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <f>G6*H6</f>
+        <v>1100</v>
+      </c>
+      <c r="J6">
+        <v>100</v>
+      </c>
+      <c r="K6">
+        <f>J6*D6</f>
+        <v>1000</v>
+      </c>
+      <c r="L6">
+        <f>G6-K6</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>90</v>
+      </c>
+      <c r="F7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7">
+        <f>E7*D7</f>
+        <v>900</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <f>G7*H7</f>
+        <v>900</v>
+      </c>
+      <c r="J7">
+        <v>100</v>
+      </c>
+      <c r="K7">
+        <f>J7*D7</f>
+        <v>1000</v>
+      </c>
+      <c r="L7">
+        <f>G7-K7</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <v>110</v>
+      </c>
+      <c r="F8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8">
+        <f>E8*D8</f>
+        <v>1100</v>
+      </c>
+      <c r="H8">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I8">
+        <f>G8*H8</f>
+        <v>1210</v>
+      </c>
+      <c r="J8">
+        <v>100</v>
+      </c>
+      <c r="K8">
+        <f>J8*D8</f>
+        <v>1000</v>
+      </c>
+      <c r="L8">
+        <f>G8-K8</f>
+        <v>100</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <f>M8*G8</f>
+        <v>1100</v>
+      </c>
+      <c r="O8">
+        <f>I8-N8</f>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <v>110</v>
+      </c>
+      <c r="F9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9">
+        <f>E9*D9</f>
+        <v>1100</v>
+      </c>
+      <c r="H9">
+        <v>0.9</v>
+      </c>
+      <c r="I9">
+        <f>G9*H9</f>
+        <v>990</v>
+      </c>
+      <c r="J9">
+        <v>100</v>
+      </c>
+      <c r="K9">
+        <f>J9*D9</f>
+        <v>1000</v>
+      </c>
+      <c r="L9">
+        <f>G9-K9</f>
+        <v>100</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <f>M9*G9</f>
+        <v>1100</v>
+      </c>
+      <c r="O9">
+        <f>I9-N9</f>
+        <v>-110</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>90</v>
+      </c>
+      <c r="F11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11">
+        <f>E11*D11</f>
+        <v>900</v>
+      </c>
+      <c r="H11">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I11">
+        <f>G11*H11</f>
+        <v>990.00000000000011</v>
+      </c>
+      <c r="J11">
+        <v>100</v>
+      </c>
+      <c r="K11">
+        <f>J11*D11</f>
+        <v>1000</v>
+      </c>
+      <c r="L11">
+        <f>G11-K11</f>
+        <v>-100</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <f>M11*G11</f>
+        <v>900</v>
+      </c>
+      <c r="O11">
+        <f>I11-N11</f>
+        <v>90.000000000000114</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+      <c r="E12">
+        <v>90</v>
+      </c>
+      <c r="F12" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12">
+        <f>E12*D12</f>
+        <v>900</v>
+      </c>
+      <c r="H12">
+        <v>0.9</v>
+      </c>
+      <c r="I12">
+        <f>G12*H12</f>
+        <v>810</v>
+      </c>
+      <c r="J12">
+        <v>100</v>
+      </c>
+      <c r="K12">
+        <f>J12*D12</f>
+        <v>1000</v>
+      </c>
+      <c r="L12">
+        <f>G12-K12</f>
+        <v>-100</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <f>M12*G12</f>
+        <v>900</v>
+      </c>
+      <c r="O12">
+        <f>I12-N12</f>
+        <v>-90</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="C16" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="M16" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="N16" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="O16" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="L17" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="O17" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="C18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18">
+        <v>1000</v>
+      </c>
+      <c r="E18">
+        <v>10</v>
+      </c>
+      <c r="F18" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18">
+        <f>E18*D18</f>
+        <v>10000</v>
+      </c>
+      <c r="H18">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I18">
+        <f>G18*H18</f>
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19">
+        <v>500</v>
+      </c>
+      <c r="E19">
+        <v>11</v>
+      </c>
+      <c r="F19" t="s">
+        <v>37</v>
+      </c>
+      <c r="G19">
+        <f>E19*D19</f>
+        <v>5500</v>
+      </c>
+      <c r="H19">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="I19">
+        <f>G19*H19</f>
+        <v>6324.9999999999991</v>
+      </c>
+      <c r="J19">
+        <v>10</v>
+      </c>
+      <c r="K19">
+        <f>J19*D19</f>
+        <v>5000</v>
+      </c>
+      <c r="L19">
+        <f>G19-K19</f>
+        <v>500</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <f>M19*G19</f>
+        <v>5500</v>
+      </c>
+      <c r="O19">
+        <f>I19-N19</f>
+        <v>824.99999999999909</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
aggiorna modifiche estensione gestione titoli
</commit_message>
<xml_diff>
--- a/report/accounting/asset_management/schema titoli.xlsx
+++ b/report/accounting/asset_management/schema titoli.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\P\Universal Images\Universal\report\accounting\asset_management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC7502D1-5FE4-4DD5-A4D2-7FDB7F09F640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9234B1C-AF8B-4AB7-A7A2-1E6ACDA7180C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29650" yWindow="1420" windowWidth="33870" windowHeight="16640" xr2:uid="{F3CD7890-2F1A-4DCC-A859-DA51742E909C}"/>
+    <workbookView xWindow="170" yWindow="1070" windowWidth="34040" windowHeight="18010" activeTab="1" xr2:uid="{F3CD7890-2F1A-4DCC-A859-DA51742E909C}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="53">
   <si>
     <t>spese</t>
   </si>
@@ -191,6 +191,9 @@
   </si>
   <si>
     <t>perdita vendita+perdita cambio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">perdita+perdita sul cambio </t>
   </si>
 </sst>
 </file>
@@ -198,7 +201,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="172" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -280,8 +283,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" indent="12"/>
     </xf>
   </cellXfs>
@@ -600,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F4E062F-3A88-4CED-BA9F-4C260A6C691F}">
   <dimension ref="C3:L45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1117,10 +1120,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A615F4CA-572D-43F0-94F7-4A07CFE4C733}">
-  <dimension ref="B2:O19"/>
+  <dimension ref="B2:O20"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1625,15 +1628,62 @@
         <v>500</v>
       </c>
       <c r="M19">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="N19">
         <f>M19*G19</f>
-        <v>5500</v>
+        <v>6050.0000000000009</v>
       </c>
       <c r="O19">
         <f>I19-N19</f>
-        <v>824.99999999999909</v>
+        <v>274.99999999999818</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20">
+        <v>500</v>
+      </c>
+      <c r="E20">
+        <v>9</v>
+      </c>
+      <c r="F20" t="s">
+        <v>37</v>
+      </c>
+      <c r="G20">
+        <f>E20*D20</f>
+        <v>4500</v>
+      </c>
+      <c r="H20">
+        <v>0.9</v>
+      </c>
+      <c r="I20">
+        <f>G20*H20</f>
+        <v>4050</v>
+      </c>
+      <c r="J20">
+        <v>10</v>
+      </c>
+      <c r="K20">
+        <f>J20*D20</f>
+        <v>5000</v>
+      </c>
+      <c r="L20">
+        <f>G20-K20</f>
+        <v>-500</v>
+      </c>
+      <c r="M20">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="N20">
+        <f>M20*G20</f>
+        <v>4950</v>
+      </c>
+      <c r="O20">
+        <f>I20-N20</f>
+        <v>-900</v>
       </c>
     </row>
   </sheetData>

</xml_diff>